<commit_message>
Validate postponement care wolf (#389)
</commit_message>
<xml_diff>
--- a/data/QALY_model/interim/postponed_healthcare/hospital_stays_costs_BE.xlsx
+++ b/data/QALY_model/interim/postponed_healthcare/hospital_stays_costs_BE.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="32">
   <si>
     <t xml:space="preserve">MDC</t>
   </si>
@@ -37,103 +37,108 @@
     <t xml:space="preserve">Reduction (%)</t>
   </si>
   <si>
-    <t xml:space="preserve">-p PRE-MDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">01 ZENUWSTELSEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">02 OOGAANDOENINGEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">03 NEUS, KEEL EN OREN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04 ADEMHALINGSSTELSEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">05 HART EN VAATSTELSEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">06 SPIJSVERTERINGSSTELSEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">07 LEVER, GAL EN PANCREAS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">08 BEWEGINGSSTELSEL EN BINDWEEFSEL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09 HUID, SUBCUTIS, BORSTKLIER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">10 ENDOCRIENE, VOEDINGS- EN STOFWISSELINGSZIEKTEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">11 NIEREN EN URINEWEGEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">12 MANNELIJKE GESLACHTSORGANEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">13 VROUWELIJKE GESLACHTSORGANEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14 ZWANGERSCHAP EN BEVALLING</t>
-  </si>
-  <si>
-    <t xml:space="preserve">15 NEONATI - PERINATALE AANDOENINGEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">16 BLOED EN BLOEDVORMENDE ORGANEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">17 MYELOPROLIFERATIEVE EN WEINIG GEDIFF. NEOPLASMATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">18 INFECTIE EN PARASITAIRE ZIEKTEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19 PSYCHISCHE STOORNISSEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20 ALCOHOL EN DRUGGEBRUIK</t>
-  </si>
-  <si>
-    <t xml:space="preserve">21 ONGEVALLEN,VERGIFTIGINGEN,TOXISCHE EFFECTEN VAN GENEESMIDDELEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">22 BRANDWONDEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23 FACTOREN DIE DE GEZONDHEID BEINVLOEDEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24 HIV INFECTIES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25 MULTIPELE TRAUMATA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FF RESTGROEP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Totaal</t>
+    <t xml:space="preserve">00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="@"/>
+    <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -153,13 +158,22 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -204,20 +218,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -238,777 +260,787 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.81"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.54"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="3" t="n">
         <v>2017</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="3" t="n">
         <v>2018</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="3" t="n">
         <v>2019</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="3" t="n">
         <v>2020</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="K1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="n">
+      <c r="B2" s="4" t="n">
         <v>3145</v>
       </c>
-      <c r="C2" s="2" t="n">
+      <c r="C2" s="4" t="n">
         <v>3131</v>
       </c>
-      <c r="D2" s="2" t="n">
+      <c r="D2" s="4" t="n">
         <v>3117</v>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E2" s="4" t="n">
         <f aca="false">AVERAGE(B2:D2)</f>
         <v>3131</v>
       </c>
-      <c r="F2" s="2" t="n">
+      <c r="F2" s="4" t="n">
         <v>3721</v>
       </c>
-      <c r="G2" s="2" t="n">
+      <c r="G2" s="4" t="n">
         <f aca="false">F2/E2*100-100</f>
         <v>18.8438198658575</v>
       </c>
-      <c r="K2" s="2"/>
+      <c r="K2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="2" t="n">
+      <c r="B3" s="4" t="n">
         <v>122281</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="4" t="n">
         <v>122004</v>
       </c>
-      <c r="D3" s="2" t="n">
+      <c r="D3" s="4" t="n">
         <v>120929</v>
       </c>
-      <c r="E3" s="2" t="n">
+      <c r="E3" s="4" t="n">
         <f aca="false">AVERAGE(B3:D3)</f>
         <v>121738</v>
       </c>
-      <c r="F3" s="2" t="n">
+      <c r="F3" s="4" t="n">
         <v>102802</v>
       </c>
-      <c r="G3" s="2" t="n">
+      <c r="G3" s="4" t="n">
         <f aca="false">F3/E3*100-100</f>
         <v>-15.5547158652188</v>
       </c>
-      <c r="K3" s="2"/>
+      <c r="K3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="n">
+      <c r="B4" s="4" t="n">
         <v>14462</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="4" t="n">
         <v>13951</v>
       </c>
-      <c r="D4" s="2" t="n">
+      <c r="D4" s="4" t="n">
         <v>14286</v>
       </c>
-      <c r="E4" s="2" t="n">
+      <c r="E4" s="4" t="n">
         <f aca="false">AVERAGE(B4:D4)</f>
         <v>14233</v>
       </c>
-      <c r="F4" s="2" t="n">
+      <c r="F4" s="4" t="n">
         <v>10662</v>
       </c>
-      <c r="G4" s="2" t="n">
+      <c r="G4" s="4" t="n">
         <f aca="false">F4/E4*100-100</f>
         <v>-25.0895805522377</v>
       </c>
-      <c r="K4" s="2"/>
+      <c r="K4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2" t="n">
+      <c r="B5" s="4" t="n">
         <v>12337</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="4" t="n">
         <v>129566</v>
       </c>
-      <c r="D5" s="2" t="n">
+      <c r="D5" s="4" t="n">
         <v>134471</v>
       </c>
-      <c r="E5" s="2" t="n">
+      <c r="E5" s="4" t="n">
         <f aca="false">AVERAGE(B5:D5)</f>
         <v>92124.6666666667</v>
       </c>
-      <c r="F5" s="2" t="n">
+      <c r="F5" s="4" t="n">
         <v>94662</v>
       </c>
-      <c r="G5" s="2" t="n">
+      <c r="G5" s="4" t="n">
         <f aca="false">F5/E5*100-100</f>
         <v>2.75423882130737</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="n">
+      <c r="B6" s="4" t="n">
         <v>144055</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="4" t="n">
         <v>147759</v>
       </c>
-      <c r="D6" s="2" t="n">
+      <c r="D6" s="4" t="n">
         <v>144816</v>
       </c>
-      <c r="E6" s="2" t="n">
+      <c r="E6" s="4" t="n">
         <f aca="false">AVERAGE(B6:D6)</f>
         <v>145543.333333333</v>
       </c>
-      <c r="F6" s="2" t="n">
+      <c r="F6" s="4" t="n">
         <v>139488</v>
       </c>
-      <c r="G6" s="2" t="n">
+      <c r="G6" s="4" t="n">
         <f aca="false">F6/E6*100-100</f>
         <v>-4.16050202688776</v>
       </c>
-      <c r="K6" s="2"/>
+      <c r="K6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="n">
+      <c r="B7" s="4" t="n">
         <v>204535</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="4" t="n">
         <v>201818</v>
       </c>
-      <c r="D7" s="2" t="n">
+      <c r="D7" s="4" t="n">
         <v>20329</v>
       </c>
-      <c r="E7" s="2" t="n">
+      <c r="E7" s="4" t="n">
         <f aca="false">AVERAGE(B7:D7)</f>
         <v>142227.333333333</v>
       </c>
-      <c r="F7" s="2" t="n">
+      <c r="F7" s="4" t="n">
         <v>170495</v>
       </c>
-      <c r="G7" s="2" t="n">
+      <c r="G7" s="4" t="n">
         <f aca="false">F7/E7*100-100</f>
         <v>19.8749888675876</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="n">
+      <c r="B8" s="4" t="n">
         <v>188652</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="4" t="n">
         <v>18.684</v>
       </c>
-      <c r="D8" s="2" t="n">
+      <c r="D8" s="4" t="n">
         <v>184727</v>
       </c>
-      <c r="E8" s="2" t="n">
+      <c r="E8" s="4" t="n">
         <f aca="false">AVERAGE(B8:D8)</f>
         <v>124465.894666667</v>
       </c>
-      <c r="F8" s="2" t="n">
+      <c r="F8" s="4" t="n">
         <v>145487</v>
       </c>
-      <c r="G8" s="2" t="n">
+      <c r="G8" s="4" t="n">
         <f aca="false">F8/E8*100-100</f>
         <v>16.8890485137556</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="n">
+      <c r="B9" s="4" t="n">
         <v>55947</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="4" t="n">
         <v>56159</v>
       </c>
-      <c r="D9" s="2" t="n">
+      <c r="D9" s="4" t="n">
         <v>57072</v>
       </c>
-      <c r="E9" s="2" t="n">
+      <c r="E9" s="4" t="n">
         <f aca="false">AVERAGE(B9:D9)</f>
         <v>56392.6666666667</v>
       </c>
-      <c r="F9" s="2" t="n">
+      <c r="F9" s="4" t="n">
         <v>51429</v>
       </c>
-      <c r="G9" s="2" t="n">
+      <c r="G9" s="4" t="n">
         <f aca="false">F9/E9*100-100</f>
         <v>-8.80197188759767</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="n">
+      <c r="B10" s="4" t="n">
         <v>254694</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="4" t="n">
         <v>253478</v>
       </c>
-      <c r="D10" s="2" t="n">
+      <c r="D10" s="4" t="n">
         <v>253659</v>
       </c>
-      <c r="E10" s="2" t="n">
+      <c r="E10" s="4" t="n">
         <f aca="false">AVERAGE(B10:D10)</f>
         <v>253943.666666667</v>
       </c>
-      <c r="F10" s="2" t="n">
+      <c r="F10" s="4" t="n">
         <v>201985</v>
       </c>
-      <c r="G10" s="2" t="n">
+      <c r="G10" s="4" t="n">
         <f aca="false">F10/E10*100-100</f>
         <v>-20.4607058520853</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="2" t="n">
+      <c r="B11" s="4" t="n">
         <v>59241</v>
       </c>
-      <c r="C11" s="2" t="n">
+      <c r="C11" s="4" t="n">
         <v>60077</v>
       </c>
-      <c r="D11" s="2" t="n">
+      <c r="D11" s="4" t="n">
         <v>60425</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="4" t="n">
         <f aca="false">AVERAGE(B11:D11)</f>
         <v>59914.3333333333</v>
       </c>
-      <c r="F11" s="2" t="n">
+      <c r="F11" s="4" t="n">
         <v>47317</v>
       </c>
-      <c r="G11" s="2" t="n">
+      <c r="G11" s="4" t="n">
         <f aca="false">F11/E11*100-100</f>
         <v>-21.0255754048836</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="2" t="n">
+      <c r="B12" s="4" t="n">
         <v>51135</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="4" t="n">
         <v>52316</v>
       </c>
-      <c r="D12" s="2" t="n">
+      <c r="D12" s="4" t="n">
         <v>49632</v>
       </c>
-      <c r="E12" s="2" t="n">
+      <c r="E12" s="4" t="n">
         <f aca="false">AVERAGE(B12:D12)</f>
         <v>51027.6666666667</v>
       </c>
-      <c r="F12" s="2" t="n">
+      <c r="F12" s="4" t="n">
         <v>39785</v>
       </c>
-      <c r="G12" s="2" t="n">
+      <c r="G12" s="4" t="n">
         <f aca="false">F12/E12*100-100</f>
         <v>-22.0324921774462</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="2" t="n">
+      <c r="B13" s="4" t="n">
         <v>83185</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="4" t="n">
         <v>86456</v>
       </c>
-      <c r="D13" s="2" t="n">
+      <c r="D13" s="4" t="n">
         <v>87407</v>
       </c>
-      <c r="E13" s="2" t="n">
+      <c r="E13" s="4" t="n">
         <f aca="false">AVERAGE(B13:D13)</f>
         <v>85682.6666666667</v>
       </c>
-      <c r="F13" s="2" t="n">
+      <c r="F13" s="4" t="n">
         <v>76300</v>
       </c>
-      <c r="G13" s="2" t="n">
+      <c r="G13" s="4" t="n">
         <f aca="false">F13/E13*100-100</f>
         <v>-10.9504839563039</v>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="2" t="n">
+      <c r="B14" s="4" t="n">
         <v>23667</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="4" t="n">
         <v>23753</v>
       </c>
-      <c r="D14" s="2" t="n">
+      <c r="D14" s="4" t="n">
         <v>24033</v>
       </c>
-      <c r="E14" s="2" t="n">
+      <c r="E14" s="4" t="n">
         <f aca="false">AVERAGE(B14:D14)</f>
         <v>23817.6666666667</v>
       </c>
-      <c r="F14" s="2" t="n">
+      <c r="F14" s="4" t="n">
         <v>1983</v>
       </c>
-      <c r="G14" s="2" t="n">
+      <c r="G14" s="4" t="n">
         <f aca="false">F14/E14*100-100</f>
         <v>-91.6742474073867</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="2" t="n">
+      <c r="B15" s="4" t="n">
         <v>31817</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="4" t="n">
         <v>31032</v>
       </c>
-      <c r="D15" s="2" t="n">
+      <c r="D15" s="4" t="n">
         <v>30777</v>
       </c>
-      <c r="E15" s="2" t="n">
+      <c r="E15" s="4" t="n">
         <f aca="false">AVERAGE(B15:D15)</f>
         <v>31208.6666666667</v>
       </c>
-      <c r="F15" s="2" t="n">
+      <c r="F15" s="4" t="n">
         <v>24035</v>
       </c>
-      <c r="G15" s="2" t="n">
+      <c r="G15" s="4" t="n">
         <f aca="false">F15/E15*100-100</f>
         <v>-22.986136329652</v>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="2" t="n">
+      <c r="B16" s="4" t="n">
         <v>135825</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="4" t="n">
         <v>135368</v>
       </c>
-      <c r="D16" s="2" t="n">
+      <c r="D16" s="4" t="n">
         <v>133889</v>
       </c>
-      <c r="E16" s="2" t="n">
+      <c r="E16" s="4" t="n">
         <f aca="false">AVERAGE(B16:D16)</f>
         <v>135027.333333333</v>
       </c>
-      <c r="F16" s="2" t="n">
+      <c r="F16" s="4" t="n">
         <v>126361</v>
       </c>
-      <c r="G16" s="2" t="n">
+      <c r="G16" s="4" t="n">
         <f aca="false">F16/E16*100-100</f>
         <v>-6.41820668407878</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="2" t="n">
+      <c r="B17" s="4" t="n">
         <v>5983</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="4" t="n">
         <v>6125</v>
       </c>
-      <c r="D17" s="2" t="n">
+      <c r="D17" s="4" t="n">
         <v>6319</v>
       </c>
-      <c r="E17" s="2" t="n">
+      <c r="E17" s="4" t="n">
         <f aca="false">AVERAGE(B17:D17)</f>
         <v>6142.33333333333</v>
       </c>
-      <c r="F17" s="2" t="n">
+      <c r="F17" s="4" t="n">
         <v>6292</v>
       </c>
-      <c r="G17" s="2" t="n">
+      <c r="G17" s="4" t="n">
         <f aca="false">F17/E17*100-100</f>
         <v>2.43664188419169</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="2" t="n">
+      <c r="B18" s="4" t="n">
         <v>16646</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="4" t="n">
         <v>1693</v>
       </c>
-      <c r="D18" s="2" t="n">
+      <c r="D18" s="4" t="n">
         <v>17378</v>
       </c>
-      <c r="E18" s="2" t="n">
+      <c r="E18" s="4" t="n">
         <f aca="false">AVERAGE(B18:D18)</f>
         <v>11905.6666666667</v>
       </c>
-      <c r="F18" s="2" t="n">
+      <c r="F18" s="4" t="n">
         <v>15181</v>
       </c>
-      <c r="G18" s="2" t="n">
+      <c r="G18" s="4" t="n">
         <f aca="false">F18/E18*100-100</f>
         <v>27.5107091861018</v>
       </c>
-      <c r="K18" s="2"/>
+      <c r="K18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="n">
+      <c r="B19" s="4" t="n">
         <v>34754</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="4" t="n">
         <v>33729</v>
       </c>
-      <c r="D19" s="2" t="n">
+      <c r="D19" s="4" t="n">
         <v>33659</v>
       </c>
-      <c r="E19" s="2" t="n">
+      <c r="E19" s="4" t="n">
         <f aca="false">AVERAGE(B19:D19)</f>
         <v>34047.3333333333</v>
       </c>
-      <c r="F19" s="2" t="n">
+      <c r="F19" s="4" t="n">
         <v>30124</v>
       </c>
-      <c r="G19" s="2" t="n">
+      <c r="G19" s="4" t="n">
         <f aca="false">F19/E19*100-100</f>
         <v>-11.5231736210374</v>
       </c>
-      <c r="K19" s="2"/>
+      <c r="K19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B20" s="2" t="n">
+      <c r="B20" s="4" t="n">
         <v>36521</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="4" t="n">
         <v>39434</v>
       </c>
-      <c r="D20" s="2" t="n">
+      <c r="D20" s="4" t="n">
         <v>39109</v>
       </c>
-      <c r="E20" s="2" t="n">
+      <c r="E20" s="4" t="n">
         <f aca="false">AVERAGE(B20:D20)</f>
         <v>38354.6666666667</v>
       </c>
-      <c r="F20" s="2" t="n">
+      <c r="F20" s="4" t="n">
         <v>32352</v>
       </c>
-      <c r="G20" s="2" t="n">
+      <c r="G20" s="4" t="n">
         <f aca="false">F20/E20*100-100</f>
         <v>-15.6504206354724</v>
       </c>
-      <c r="K20" s="2"/>
+      <c r="K20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B21" s="2" t="n">
+      <c r="B21" s="4" t="n">
         <v>23283</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="4" t="n">
         <v>23264</v>
       </c>
-      <c r="D21" s="2" t="n">
+      <c r="D21" s="4" t="n">
         <v>22994</v>
       </c>
-      <c r="E21" s="2" t="n">
+      <c r="E21" s="4" t="n">
         <f aca="false">AVERAGE(B21:D21)</f>
         <v>23180.3333333333</v>
       </c>
-      <c r="F21" s="2" t="n">
+      <c r="F21" s="4" t="n">
         <v>17278</v>
       </c>
-      <c r="G21" s="2" t="n">
+      <c r="G21" s="4" t="n">
         <f aca="false">F21/E21*100-100</f>
         <v>-25.4626766943242</v>
       </c>
-      <c r="K21" s="2"/>
+      <c r="K21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B22" s="2" t="n">
+      <c r="B22" s="4" t="n">
         <v>1207</v>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C22" s="4" t="n">
         <v>11892</v>
       </c>
-      <c r="D22" s="2" t="n">
+      <c r="D22" s="4" t="n">
         <v>12139</v>
       </c>
-      <c r="E22" s="2" t="n">
+      <c r="E22" s="4" t="n">
         <f aca="false">AVERAGE(B22:D22)</f>
         <v>8412.66666666667</v>
       </c>
-      <c r="F22" s="2" t="n">
+      <c r="F22" s="4" t="n">
         <v>9083</v>
       </c>
-      <c r="G22" s="2" t="n">
+      <c r="G22" s="4" t="n">
         <f aca="false">F22/E22*100-100</f>
         <v>7.96814327601237</v>
       </c>
-      <c r="K22" s="2"/>
+      <c r="K22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="2" t="n">
+      <c r="B23" s="4" t="n">
         <v>24894</v>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="C23" s="4" t="n">
         <v>25448</v>
       </c>
-      <c r="D23" s="2" t="n">
+      <c r="D23" s="4" t="n">
         <v>25407</v>
       </c>
-      <c r="E23" s="2" t="n">
+      <c r="E23" s="4" t="n">
         <f aca="false">AVERAGE(B23:D23)</f>
         <v>25249.6666666667</v>
       </c>
-      <c r="F23" s="2" t="n">
+      <c r="F23" s="4" t="n">
         <v>20133</v>
       </c>
-      <c r="G23" s="2" t="n">
+      <c r="G23" s="4" t="n">
         <f aca="false">F23/E23*100-100</f>
         <v>-20.2642939180715</v>
       </c>
-      <c r="K23" s="2"/>
+      <c r="K23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B24" s="2" t="n">
+      <c r="B24" s="4" t="n">
         <v>947</v>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="C24" s="4" t="n">
         <v>931</v>
       </c>
-      <c r="D24" s="2" t="n">
+      <c r="D24" s="4" t="n">
         <v>893</v>
       </c>
-      <c r="E24" s="2" t="n">
+      <c r="E24" s="4" t="n">
         <f aca="false">AVERAGE(B24:D24)</f>
         <v>923.666666666667</v>
       </c>
-      <c r="F24" s="2" t="n">
+      <c r="F24" s="4" t="n">
         <v>697</v>
       </c>
-      <c r="G24" s="2" t="n">
+      <c r="G24" s="4" t="n">
         <f aca="false">F24/E24*100-100</f>
         <v>-24.5398773006135</v>
       </c>
-      <c r="K24" s="2"/>
+      <c r="K24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2" t="n">
+      <c r="B25" s="4" t="n">
         <v>63562</v>
       </c>
-      <c r="C25" s="2" t="n">
+      <c r="C25" s="4" t="n">
         <v>60788</v>
       </c>
-      <c r="D25" s="2" t="n">
+      <c r="D25" s="4" t="n">
         <v>59837</v>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="4" t="n">
         <f aca="false">AVERAGE(B25:D25)</f>
         <v>61395.6666666667</v>
       </c>
-      <c r="F25" s="2" t="n">
+      <c r="F25" s="4" t="n">
         <v>44989</v>
       </c>
-      <c r="G25" s="2" t="n">
+      <c r="G25" s="4" t="n">
         <f aca="false">F25/E25*100-100</f>
         <v>-26.7228414600379</v>
       </c>
-      <c r="K25" s="2"/>
+      <c r="K25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2" t="n">
+      <c r="B26" s="4" t="n">
         <v>720</v>
       </c>
-      <c r="C26" s="2" t="n">
+      <c r="C26" s="4" t="n">
         <v>741</v>
       </c>
-      <c r="D26" s="2" t="n">
+      <c r="D26" s="4" t="n">
         <v>757</v>
       </c>
-      <c r="E26" s="2" t="n">
+      <c r="E26" s="4" t="n">
         <f aca="false">AVERAGE(B26:D26)</f>
         <v>739.333333333333</v>
       </c>
-      <c r="F26" s="2" t="n">
+      <c r="F26" s="4" t="n">
         <v>643</v>
       </c>
-      <c r="G26" s="2" t="n">
+      <c r="G26" s="4" t="n">
         <f aca="false">F26/E26*100-100</f>
         <v>-13.0297565374211</v>
       </c>
-      <c r="K26" s="2"/>
+      <c r="K26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2" t="n">
+      <c r="B27" s="4" t="n">
         <v>2634</v>
       </c>
-      <c r="C27" s="2" t="n">
+      <c r="C27" s="4" t="n">
         <v>2727</v>
       </c>
-      <c r="D27" s="2" t="n">
+      <c r="D27" s="4" t="n">
         <v>2798</v>
       </c>
-      <c r="E27" s="2" t="n">
+      <c r="E27" s="4" t="n">
         <f aca="false">AVERAGE(B27:D27)</f>
         <v>2719.66666666667</v>
       </c>
-      <c r="F27" s="2" t="n">
+      <c r="F27" s="4" t="n">
         <v>2642</v>
       </c>
-      <c r="G27" s="2" t="n">
+      <c r="G27" s="4" t="n">
         <f aca="false">F27/E27*100-100</f>
         <v>-2.85574212526043</v>
       </c>
-      <c r="K27" s="2"/>
+      <c r="K27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="2" t="n">
+      <c r="B28" s="0"/>
+      <c r="K28" s="4"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="4" t="n">
         <v>23434</v>
       </c>
-      <c r="C28" s="2" t="n">
+      <c r="C29" s="4" t="n">
         <v>23786</v>
       </c>
-      <c r="D28" s="2" t="n">
+      <c r="D29" s="4" t="n">
         <v>22235</v>
       </c>
-      <c r="E28" s="2" t="n">
-        <f aca="false">AVERAGE(B28:D28)</f>
+      <c r="E29" s="4" t="n">
+        <f aca="false">AVERAGE(B29:D29)</f>
         <v>23151.6666666667</v>
       </c>
-      <c r="F28" s="2" t="n">
+      <c r="F29" s="4" t="n">
         <v>20087</v>
       </c>
-      <c r="G28" s="2" t="n">
-        <f aca="false">F28/E28*100-100</f>
+      <c r="G29" s="4" t="n">
+        <f aca="false">F29/E29*100-100</f>
         <v>-13.2373479231157</v>
       </c>
-      <c r="K28" s="2"/>
-    </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B29" s="2" t="n">
+      <c r="K29" s="4"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="4" t="n">
         <f aca="false">SUM(B2:B28)</f>
-        <v>1619563</v>
-      </c>
-      <c r="C29" s="2" t="n">
+        <v>1596129</v>
+      </c>
+      <c r="C30" s="4" t="n">
         <f aca="false">SUM(C2:C28)</f>
-        <v>1547444.684</v>
-      </c>
-      <c r="D29" s="2" t="n">
+        <v>1523658.684</v>
+      </c>
+      <c r="D30" s="4" t="n">
         <f aca="false">SUM(D2:D28)</f>
-        <v>1563094</v>
-      </c>
-      <c r="E29" s="2" t="n">
-        <f aca="false">AVERAGE(B29:D29)</f>
-        <v>1576700.56133333</v>
-      </c>
-      <c r="F29" s="2" t="n">
+        <v>1540859</v>
+      </c>
+      <c r="E30" s="4" t="n">
+        <f aca="false">AVERAGE(B30:D30)</f>
+        <v>1553548.89466667</v>
+      </c>
+      <c r="F30" s="4" t="n">
         <f aca="false">SUM(F2:F28)</f>
-        <v>1436013</v>
-      </c>
-      <c r="G29" s="3" t="n">
-        <f aca="false">F29/E29*100-100</f>
-        <v>-8.92290931984962</v>
-      </c>
-      <c r="K29" s="2"/>
+        <v>1415926</v>
+      </c>
+      <c r="G30" s="5" t="n">
+        <f aca="false">F30/E30*100-100</f>
+        <v>-8.858613664438</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1021,34 +1053,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H36" activeCellId="0" sqref="H36"/>
+      <selection pane="topLeft" activeCell="I29" activeCellId="0" sqref="I29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="n">
+      <c r="B1" s="3" t="n">
         <v>2017</v>
       </c>
-      <c r="C1" s="1" t="n">
+      <c r="C1" s="3" t="n">
         <v>2018</v>
       </c>
-      <c r="D1" s="1" t="n">
+      <c r="D1" s="3" t="n">
         <v>2019</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="n">
+      <c r="F1" s="3" t="n">
         <v>2020</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1057,24 +1089,24 @@
         <v>3</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>177422869.39</v>
+        <v>265569046.66</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>178239905.02</v>
+        <v>274564496.27</v>
       </c>
       <c r="D2" s="0" t="n">
-        <v>181182840.25</v>
+        <v>266167726.51</v>
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">AVERAGE(B2:D2)</f>
-        <v>178948538.22</v>
+        <v>268767089.813333</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>220478749.51</v>
+        <v>266036419.1</v>
       </c>
       <c r="G2" s="0" t="n">
         <f aca="false">F2/E2*100-100</f>
-        <v>23.2079075376087</v>
+        <v>-1.01599891386624</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1474,7 +1506,7 @@
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">F18/E18*100-100</f>
-        <v>-1.58143685675469</v>
+        <v>-1.58143685675468</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1706,60 +1738,65 @@
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="0" t="n">
-        <v>265569046.66</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>274564496.27</v>
-      </c>
-      <c r="D28" s="0" t="n">
-        <v>266167726.51</v>
-      </c>
-      <c r="E28" s="0" t="n">
-        <f aca="false">AVERAGE(B28:D28)</f>
-        <v>268767089.813333</v>
-      </c>
-      <c r="F28" s="0" t="n">
-        <v>266036419.1</v>
-      </c>
-      <c r="G28" s="0" t="n">
-        <f aca="false">F28/E28*100-100</f>
-        <v>-1.01599891386624</v>
-      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="0" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="0" t="n">
-        <f aca="false">SUM(B2:B28)</f>
-        <v>8882583880.89</v>
+        <v>177422869.39</v>
       </c>
       <c r="C29" s="0" t="n">
-        <f aca="false">SUM(C2:C28)</f>
-        <v>9058321482.39</v>
+        <v>178239905.02</v>
       </c>
       <c r="D29" s="0" t="n">
-        <f aca="false">SUM(D2:D28)</f>
-        <v>9274376587.23</v>
+        <v>181182840.25</v>
       </c>
       <c r="E29" s="0" t="n">
         <f aca="false">AVERAGE(B29:D29)</f>
-        <v>9071760650.17</v>
+        <v>178948538.22</v>
       </c>
       <c r="F29" s="0" t="n">
-        <f aca="false">SUM(F2:F28)</f>
-        <v>8332846345.98</v>
+        <v>220478749.51</v>
       </c>
       <c r="G29" s="0" t="n">
         <f aca="false">F29/E29*100-100</f>
-        <v>-8.14521384199166</v>
+        <v>23.2079075376087</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <f aca="false">SUM(B2:B28)</f>
+        <v>8705161011.5</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <f aca="false">SUM(C2:C28)</f>
+        <v>8880081577.37</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <f aca="false">SUM(D2:D28)</f>
+        <v>9093193746.98</v>
+      </c>
+      <c r="E30" s="0" t="n">
+        <f aca="false">AVERAGE(B30:D30)</f>
+        <v>8892812111.95</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <f aca="false">SUM(F2:F28)</f>
+        <v>8112367596.47</v>
+      </c>
+      <c r="G30" s="0" t="n">
+        <f aca="false">F30/E30*100-100</f>
+        <v>-8.77612734481652</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>